<commit_message>
info.xlsx 2021 12 8
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_get_lesson_pic_recognize\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codehub\Automatic_grab_class_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6501754D-A6AF-4C11-8148-C13C7864A84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722939A0-93A9-476D-94B8-D3E544D7BA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,18 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>事件描述（想写就写）</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>待点击图标名/等待的时间(秒)/输入的字符串/热键</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>单击重复次数（不写为1，死循环为-1）</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>baidu.png</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -47,60 +35,27 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>操作类型：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="10"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1.左键单击      2.输入字符串       3.等待</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4.热键</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>back.png</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>事件描述（想写就写）</t>
+  </si>
+  <si>
+    <t>操作类型：1.左键单击（循环直到找到图片为止）      2.输入字符串       3.等待      4.热键      5.左键单击（无需找到图片）</t>
+  </si>
+  <si>
+    <t>待点击图标名/等待的时间(秒)/输入的字符串/热键</t>
+  </si>
+  <si>
+    <t>单击重复次数（不写为1，死循环为-1）</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,20 +92,19 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="10"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -165,9 +119,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -451,29 +407,29 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="116" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -481,7 +437,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -489,7 +445,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -497,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>